<commit_message>
add stats vs Eagles
</commit_message>
<xml_diff>
--- a/public/statistic/teams-position.xlsx
+++ b/public/statistic/teams-position.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Баскетбол\Отчёты\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2AC4B581-0968-425B-9AF3-AA8AA2B03626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ACFC9924-9C83-40BD-A632-54129D056171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{EEBDC336-3292-4C62-B3E8-FB0F229B6B8F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{492D5077-27FF-4743-9712-165EC8A8B88E}"/>
   </bookViews>
   <sheets>
     <sheet name="Д3" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Д3</t>
   </si>
@@ -51,88 +51,88 @@
     <t>Очки</t>
   </si>
   <si>
+    <t>GOLDEN HILL</t>
+  </si>
+  <si>
+    <t>285 - 240</t>
+  </si>
+  <si>
+    <t>ISsoft</t>
+  </si>
+  <si>
+    <t>235 - 214</t>
+  </si>
+  <si>
+    <t>Грушвиль</t>
+  </si>
+  <si>
+    <t>317 - 262</t>
+  </si>
+  <si>
     <t>Эра-Недвижимости плюс</t>
   </si>
   <si>
-    <t>233 - 173</t>
-  </si>
-  <si>
-    <t>GOLDEN HILL</t>
-  </si>
-  <si>
-    <t>199 - 171</t>
-  </si>
-  <si>
-    <t>ISsoft</t>
-  </si>
-  <si>
-    <t>162 - 154</t>
-  </si>
-  <si>
-    <t>Грушвиль</t>
-  </si>
-  <si>
-    <t>241 - 192</t>
+    <t>293 - 246</t>
   </si>
   <si>
     <t>БГУФК</t>
   </si>
   <si>
-    <t>186 - 140</t>
+    <t>239 - 199</t>
+  </si>
+  <si>
+    <t>VSS</t>
+  </si>
+  <si>
+    <t>246 - 257</t>
+  </si>
+  <si>
+    <t>ОПЛАТИ</t>
+  </si>
+  <si>
+    <t>258 - 239</t>
+  </si>
+  <si>
+    <t>SIRIUS</t>
+  </si>
+  <si>
+    <t>257 - 234</t>
+  </si>
+  <si>
+    <t>Стрела</t>
+  </si>
+  <si>
+    <t>254 - 267</t>
   </si>
   <si>
     <t>Mapogo males</t>
   </si>
   <si>
-    <t>158 - 145</t>
-  </si>
-  <si>
-    <t>Стрела</t>
-  </si>
-  <si>
-    <t>189 - 201</t>
-  </si>
-  <si>
-    <t>SIRIUS</t>
-  </si>
-  <si>
-    <t>209 - 192</t>
+    <t>227 - 231</t>
+  </si>
+  <si>
+    <t>NORD</t>
+  </si>
+  <si>
+    <t>201 - 354</t>
+  </si>
+  <si>
+    <t>Eagles</t>
+  </si>
+  <si>
+    <t>214 - 222</t>
   </si>
   <si>
     <t>ЛФК</t>
   </si>
   <si>
-    <t>170 - 192</t>
-  </si>
-  <si>
-    <t>ОПЛАТИ</t>
-  </si>
-  <si>
-    <t>195 - 191</t>
-  </si>
-  <si>
-    <t>Eagles</t>
-  </si>
-  <si>
-    <t>172 - 174</t>
-  </si>
-  <si>
-    <t>VSS</t>
-  </si>
-  <si>
-    <t>187 - 204</t>
-  </si>
-  <si>
-    <t>NORD</t>
-  </si>
-  <si>
-    <t>135 - 289</t>
+    <t>240 - 268</t>
   </si>
   <si>
     <t>Минск 7х</t>
   </si>
   <si>
-    <t>101 - 119</t>
+    <t>149 - 182</t>
   </si>
   <si>
     <t>Стрела - Mapogo males 75:81 (16:30, БНТУ)</t>
@@ -193,6 +193,27 @@
   </si>
   <si>
     <t>Стрела - ОПЛАТИ 61:72 (15:30, БНТУ)</t>
+  </si>
+  <si>
+    <t>ЛФК - Грушвиль 70:76 (16:30, БНТУ)</t>
+  </si>
+  <si>
+    <t>ОПЛАТИ - Минск 7х 63:48 (18:00, БНТУ)</t>
+  </si>
+  <si>
+    <t>VSS - БГУФК 59:53 (19:30, БНТУ)</t>
+  </si>
+  <si>
+    <t>NORD - Стрела 66:65 (11:00, БНТУ)</t>
+  </si>
+  <si>
+    <t>GOLDEN HILL - Mapogo males 86:69 (12:30, БНТУ)</t>
+  </si>
+  <si>
+    <t>ISsoft - Эра-Недвижимости плюс 73:60 (14:00, БНТУ)</t>
+  </si>
+  <si>
+    <t>Eagles - SIRIUS 42:48 (15:30, БНТУ)</t>
   </si>
 </sst>
 </file>
@@ -648,8 +669,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4019C1D4-CC22-47F5-A42A-749B80A0020F}">
-  <dimension ref="B2:H45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97FF6154-EA29-455B-A5E0-DD959281605B}">
+  <dimension ref="B2:H54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -704,10 +725,10 @@
         <v>8</v>
       </c>
       <c r="D5" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E5" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F5" s="3">
         <v>0</v>
@@ -716,7 +737,7 @@
         <v>9</v>
       </c>
       <c r="H5" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -727,19 +748,19 @@
         <v>10</v>
       </c>
       <c r="D6" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E6" s="5">
         <v>3</v>
       </c>
       <c r="F6" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>11</v>
       </c>
       <c r="H6" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -750,10 +771,10 @@
         <v>12</v>
       </c>
       <c r="D7" s="5">
+        <v>4</v>
+      </c>
+      <c r="E7" s="5">
         <v>3</v>
-      </c>
-      <c r="E7" s="5">
-        <v>2</v>
       </c>
       <c r="F7" s="5">
         <v>1</v>
@@ -762,7 +783,7 @@
         <v>13</v>
       </c>
       <c r="H7" s="5">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -773,10 +794,10 @@
         <v>14</v>
       </c>
       <c r="D8" s="5">
+        <v>4</v>
+      </c>
+      <c r="E8" s="5">
         <v>3</v>
-      </c>
-      <c r="E8" s="5">
-        <v>2</v>
       </c>
       <c r="F8" s="5">
         <v>1</v>
@@ -785,7 +806,7 @@
         <v>15</v>
       </c>
       <c r="H8" s="5">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -796,19 +817,19 @@
         <v>16</v>
       </c>
       <c r="D9" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E9" s="5">
         <v>2</v>
       </c>
       <c r="F9" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>17</v>
       </c>
       <c r="H9" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -819,19 +840,19 @@
         <v>18</v>
       </c>
       <c r="D10" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E10" s="5">
         <v>2</v>
       </c>
       <c r="F10" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H10" s="5">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -842,10 +863,10 @@
         <v>20</v>
       </c>
       <c r="D11" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E11" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F11" s="5">
         <v>2</v>
@@ -854,7 +875,7 @@
         <v>21</v>
       </c>
       <c r="H11" s="5">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -865,10 +886,10 @@
         <v>22</v>
       </c>
       <c r="D12" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E12" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12" s="5">
         <v>2</v>
@@ -877,7 +898,7 @@
         <v>23</v>
       </c>
       <c r="H12" s="5">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -888,19 +909,19 @@
         <v>24</v>
       </c>
       <c r="D13" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E13" s="7">
         <v>1</v>
       </c>
       <c r="F13" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>25</v>
       </c>
       <c r="H13" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -914,16 +935,16 @@
         <v>3</v>
       </c>
       <c r="E14" s="7">
+        <v>2</v>
+      </c>
+      <c r="F14" s="7">
         <v>1</v>
-      </c>
-      <c r="F14" s="7">
-        <v>2</v>
       </c>
       <c r="G14" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H14" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -934,19 +955,19 @@
         <v>28</v>
       </c>
       <c r="D15" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E15" s="7">
         <v>1</v>
       </c>
       <c r="F15" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>29</v>
       </c>
       <c r="H15" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -957,19 +978,19 @@
         <v>30</v>
       </c>
       <c r="D16" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E16" s="7">
         <v>1</v>
       </c>
       <c r="F16" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G16" s="7" t="s">
         <v>31</v>
       </c>
       <c r="H16" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -980,10 +1001,10 @@
         <v>32</v>
       </c>
       <c r="D17" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E17" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="7">
         <v>3</v>
@@ -992,7 +1013,7 @@
         <v>33</v>
       </c>
       <c r="H17" s="7">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1003,19 +1024,19 @@
         <v>34</v>
       </c>
       <c r="D18" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E18" s="7">
         <v>0</v>
       </c>
       <c r="F18" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H18" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
@@ -1304,11 +1325,119 @@
       <c r="G45" s="11"/>
       <c r="H45" s="11"/>
     </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B46" s="10">
+        <v>45612</v>
+      </c>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+    </row>
+    <row r="47" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+    </row>
+    <row r="48" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+    </row>
+    <row r="49" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B50" s="10">
+        <v>45613</v>
+      </c>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="9"/>
+    </row>
+    <row r="51" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+    </row>
+    <row r="52" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="11"/>
+      <c r="G52" s="11"/>
+      <c r="H52" s="11"/>
+    </row>
+    <row r="53" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C53" s="11"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11"/>
+    </row>
+    <row r="54" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C54" s="11"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="11"/>
+      <c r="F54" s="11"/>
+      <c r="G54" s="11"/>
+      <c r="H54" s="11"/>
+    </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="36">
+    <mergeCell ref="B49:H49"/>
+    <mergeCell ref="B50:H50"/>
+    <mergeCell ref="B51:H51"/>
+    <mergeCell ref="B52:H52"/>
+    <mergeCell ref="B53:H53"/>
+    <mergeCell ref="B54:H54"/>
     <mergeCell ref="B43:H43"/>
     <mergeCell ref="B44:H44"/>
     <mergeCell ref="B45:H45"/>
+    <mergeCell ref="B46:H46"/>
+    <mergeCell ref="B47:H47"/>
+    <mergeCell ref="B48:H48"/>
     <mergeCell ref="B37:H37"/>
     <mergeCell ref="B38:H38"/>
     <mergeCell ref="B39:H39"/>

</xml_diff>

<commit_message>
add stats vs Oplati
</commit_message>
<xml_diff>
--- a/public/statistic/teams-position.xlsx
+++ b/public/statistic/teams-position.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Баскетбол\Отчёты\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ACFC9924-9C83-40BD-A632-54129D056171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{451AC202-3736-4870-A966-5EA4ECF05CAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{492D5077-27FF-4743-9712-165EC8A8B88E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0A5AA39C-B10B-4F7B-B83F-4D65246B8E2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Д3" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>Д3</t>
   </si>
@@ -54,85 +54,85 @@
     <t>GOLDEN HILL</t>
   </si>
   <si>
-    <t>285 - 240</t>
+    <t>357 - 306</t>
   </si>
   <si>
     <t>ISsoft</t>
   </si>
   <si>
-    <t>235 - 214</t>
+    <t>291 - 256</t>
+  </si>
+  <si>
+    <t>Эра-Недвижимости плюс</t>
+  </si>
+  <si>
+    <t>373 - 310</t>
   </si>
   <si>
     <t>Грушвиль</t>
   </si>
   <si>
-    <t>317 - 262</t>
-  </si>
-  <si>
-    <t>Эра-Недвижимости плюс</t>
-  </si>
-  <si>
-    <t>293 - 246</t>
+    <t>391 - 332</t>
+  </si>
+  <si>
+    <t>ОПЛАТИ</t>
+  </si>
+  <si>
+    <t>318 - 288</t>
   </si>
   <si>
     <t>БГУФК</t>
   </si>
   <si>
-    <t>239 - 199</t>
+    <t>309 - 273</t>
+  </si>
+  <si>
+    <t>Mapogo males</t>
+  </si>
+  <si>
+    <t>296 - 284</t>
   </si>
   <si>
     <t>VSS</t>
   </si>
   <si>
-    <t>246 - 257</t>
-  </si>
-  <si>
-    <t>ОПЛАТИ</t>
-  </si>
-  <si>
-    <t>258 - 239</t>
+    <t>310 - 337</t>
   </si>
   <si>
     <t>SIRIUS</t>
   </si>
   <si>
-    <t>257 - 234</t>
+    <t>306 - 294</t>
+  </si>
+  <si>
+    <t>NORD</t>
+  </si>
+  <si>
+    <t>254 - 395</t>
   </si>
   <si>
     <t>Стрела</t>
   </si>
   <si>
-    <t>254 - 267</t>
-  </si>
-  <si>
-    <t>Mapogo males</t>
-  </si>
-  <si>
-    <t>227 - 231</t>
-  </si>
-  <si>
-    <t>NORD</t>
-  </si>
-  <si>
-    <t>201 - 354</t>
+    <t>296 - 323</t>
   </si>
   <si>
     <t>Eagles</t>
   </si>
   <si>
-    <t>214 - 222</t>
+    <t>280 - 294</t>
   </si>
   <si>
     <t>ЛФК</t>
   </si>
   <si>
-    <t>240 - 268</t>
+    <t>293 - 337</t>
   </si>
   <si>
     <t>Минск 7х</t>
   </si>
   <si>
-    <t>149 - 182</t>
+    <t>190 - 235</t>
   </si>
   <si>
     <t>Стрела - Mapogo males 75:81 (16:30, БНТУ)</t>
@@ -214,6 +214,27 @@
   </si>
   <si>
     <t>Eagles - SIRIUS 42:48 (15:30, БНТУ)</t>
+  </si>
+  <si>
+    <t>Грушвиль - БГУФК 74:70 (16:30, БНТУ)</t>
+  </si>
+  <si>
+    <t>Стрела - ISsoft 42:56 (18:00, БНТУ)</t>
+  </si>
+  <si>
+    <t>Mapogo males - ЛФК 69:53 (19:30, БНТУ)</t>
+  </si>
+  <si>
+    <t>Минск 7х - NORD 41:53 (11:00, БНТУ)</t>
+  </si>
+  <si>
+    <t>Эра-Недвижимости плюс - VSS 80:64 (12:30, БНТУ)</t>
+  </si>
+  <si>
+    <t>GOLDEN HILL - Eagles 72:66 (14:00, БНТУ)</t>
+  </si>
+  <si>
+    <t>SIRIUS - ОПЛАТИ 49:60 (15:30, БНТУ)</t>
   </si>
 </sst>
 </file>
@@ -669,8 +690,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97FF6154-EA29-455B-A5E0-DD959281605B}">
-  <dimension ref="B2:H54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC2E33EB-FC42-469D-B54A-15D2E49BD7AD}">
+  <dimension ref="B2:H63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -725,10 +746,10 @@
         <v>8</v>
       </c>
       <c r="D5" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E5" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F5" s="3">
         <v>0</v>
@@ -737,7 +758,7 @@
         <v>9</v>
       </c>
       <c r="H5" s="3">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -748,10 +769,10 @@
         <v>10</v>
       </c>
       <c r="D6" s="5">
+        <v>5</v>
+      </c>
+      <c r="E6" s="5">
         <v>4</v>
-      </c>
-      <c r="E6" s="5">
-        <v>3</v>
       </c>
       <c r="F6" s="5">
         <v>1</v>
@@ -760,7 +781,7 @@
         <v>11</v>
       </c>
       <c r="H6" s="5">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -771,10 +792,10 @@
         <v>12</v>
       </c>
       <c r="D7" s="5">
+        <v>5</v>
+      </c>
+      <c r="E7" s="5">
         <v>4</v>
-      </c>
-      <c r="E7" s="5">
-        <v>3</v>
       </c>
       <c r="F7" s="5">
         <v>1</v>
@@ -783,7 +804,7 @@
         <v>13</v>
       </c>
       <c r="H7" s="5">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -794,10 +815,10 @@
         <v>14</v>
       </c>
       <c r="D8" s="5">
+        <v>5</v>
+      </c>
+      <c r="E8" s="5">
         <v>4</v>
-      </c>
-      <c r="E8" s="5">
-        <v>3</v>
       </c>
       <c r="F8" s="5">
         <v>1</v>
@@ -806,7 +827,7 @@
         <v>15</v>
       </c>
       <c r="H8" s="5">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -817,10 +838,10 @@
         <v>16</v>
       </c>
       <c r="D9" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E9" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F9" s="5">
         <v>2</v>
@@ -829,7 +850,7 @@
         <v>17</v>
       </c>
       <c r="H9" s="5">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -840,19 +861,19 @@
         <v>18</v>
       </c>
       <c r="D10" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E10" s="5">
         <v>2</v>
       </c>
       <c r="F10" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H10" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -866,16 +887,16 @@
         <v>4</v>
       </c>
       <c r="E11" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F11" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>21</v>
       </c>
       <c r="H11" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -886,19 +907,19 @@
         <v>22</v>
       </c>
       <c r="D12" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E12" s="5">
         <v>2</v>
       </c>
       <c r="F12" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H12" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -909,10 +930,10 @@
         <v>24</v>
       </c>
       <c r="D13" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E13" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13" s="7">
         <v>3</v>
@@ -921,7 +942,7 @@
         <v>25</v>
       </c>
       <c r="H13" s="7">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -932,19 +953,19 @@
         <v>26</v>
       </c>
       <c r="D14" s="7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E14" s="7">
         <v>2</v>
       </c>
       <c r="F14" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G14" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H14" s="7">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -955,19 +976,19 @@
         <v>28</v>
       </c>
       <c r="D15" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E15" s="7">
         <v>1</v>
       </c>
       <c r="F15" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>29</v>
       </c>
       <c r="H15" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -978,19 +999,19 @@
         <v>30</v>
       </c>
       <c r="D16" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E16" s="7">
         <v>1</v>
       </c>
       <c r="F16" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G16" s="7" t="s">
         <v>31</v>
       </c>
       <c r="H16" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1001,19 +1022,19 @@
         <v>32</v>
       </c>
       <c r="D17" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E17" s="7">
         <v>1</v>
       </c>
       <c r="F17" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>33</v>
       </c>
       <c r="H17" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1024,19 +1045,19 @@
         <v>34</v>
       </c>
       <c r="D18" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E18" s="7">
         <v>0</v>
       </c>
       <c r="F18" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H18" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
@@ -1424,8 +1445,116 @@
       <c r="G54" s="11"/>
       <c r="H54" s="11"/>
     </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B55" s="10">
+        <v>45626</v>
+      </c>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
+      <c r="G55" s="9"/>
+      <c r="H55" s="9"/>
+    </row>
+    <row r="56" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11"/>
+    </row>
+    <row r="57" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C57" s="11"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
+    </row>
+    <row r="58" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C58" s="11"/>
+      <c r="D58" s="11"/>
+      <c r="E58" s="11"/>
+      <c r="F58" s="11"/>
+      <c r="G58" s="11"/>
+      <c r="H58" s="11"/>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B59" s="10">
+        <v>45627</v>
+      </c>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
+      <c r="G59" s="9"/>
+      <c r="H59" s="9"/>
+    </row>
+    <row r="60" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C60" s="11"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="11"/>
+      <c r="F60" s="11"/>
+      <c r="G60" s="11"/>
+      <c r="H60" s="11"/>
+    </row>
+    <row r="61" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C61" s="11"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="11"/>
+      <c r="G61" s="11"/>
+      <c r="H61" s="11"/>
+    </row>
+    <row r="62" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C62" s="11"/>
+      <c r="D62" s="11"/>
+      <c r="E62" s="11"/>
+      <c r="F62" s="11"/>
+      <c r="G62" s="11"/>
+      <c r="H62" s="11"/>
+    </row>
+    <row r="63" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C63" s="11"/>
+      <c r="D63" s="11"/>
+      <c r="E63" s="11"/>
+      <c r="F63" s="11"/>
+      <c r="G63" s="11"/>
+      <c r="H63" s="11"/>
+    </row>
   </sheetData>
-  <mergeCells count="36">
+  <mergeCells count="45">
+    <mergeCell ref="B61:H61"/>
+    <mergeCell ref="B62:H62"/>
+    <mergeCell ref="B63:H63"/>
+    <mergeCell ref="B55:H55"/>
+    <mergeCell ref="B56:H56"/>
+    <mergeCell ref="B57:H57"/>
+    <mergeCell ref="B58:H58"/>
+    <mergeCell ref="B59:H59"/>
+    <mergeCell ref="B60:H60"/>
     <mergeCell ref="B49:H49"/>
     <mergeCell ref="B50:H50"/>
     <mergeCell ref="B51:H51"/>

</xml_diff>

<commit_message>
add stats vs ISsoft
</commit_message>
<xml_diff>
--- a/public/statistic/teams-position.xlsx
+++ b/public/statistic/teams-position.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Баскетбол\Отчёты\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA0EFBFA-634B-43D0-BC37-5A92C9BBD522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{04DAFCBA-60C5-45F8-8143-6A53D88BE39D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FFB953D9-EE53-4BEE-8DA1-773BEB36BC3D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CE9FB605-9350-4803-900F-F452311DAEA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Д3" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <si>
     <t>Д3</t>
   </si>
@@ -51,88 +51,88 @@
     <t>Очки</t>
   </si>
   <si>
+    <t>GOLDEN HILL</t>
+  </si>
+  <si>
+    <t>498 - 433</t>
+  </si>
+  <si>
+    <t>Эра-Недвижимости плюс</t>
+  </si>
+  <si>
+    <t>532 - 455</t>
+  </si>
+  <si>
     <t>ISsoft</t>
   </si>
   <si>
-    <t>373 - 305</t>
-  </si>
-  <si>
-    <t>GOLDEN HILL</t>
-  </si>
-  <si>
-    <t>430 - 388</t>
-  </si>
-  <si>
-    <t>Эра-Недвижимости плюс</t>
-  </si>
-  <si>
-    <t>443 - 363</t>
+    <t>426 - 372</t>
+  </si>
+  <si>
+    <t>ОПЛАТИ</t>
+  </si>
+  <si>
+    <t>489 - 437</t>
+  </si>
+  <si>
+    <t>Грушвиль</t>
+  </si>
+  <si>
+    <t>520 - 461</t>
   </si>
   <si>
     <t>Mapogo males</t>
   </si>
   <si>
-    <t>445 - 397</t>
-  </si>
-  <si>
-    <t>Грушвиль</t>
-  </si>
-  <si>
-    <t>444 - 402</t>
-  </si>
-  <si>
-    <t>ОПЛАТИ</t>
-  </si>
-  <si>
-    <t>400 - 361</t>
+    <t>521 - 486</t>
   </si>
   <si>
     <t>БГУФК</t>
   </si>
   <si>
-    <t>405 - 323</t>
+    <t>497 - 412</t>
   </si>
   <si>
     <t>SIRIUS</t>
   </si>
   <si>
-    <t>391 - 338</t>
+    <t>458 - 391</t>
+  </si>
+  <si>
+    <t>VSS</t>
+  </si>
+  <si>
+    <t>437 - 438</t>
   </si>
   <si>
     <t>Стрела</t>
   </si>
   <si>
-    <t>368 - 382</t>
+    <t>427 - 458</t>
   </si>
   <si>
     <t>NORD</t>
   </si>
   <si>
-    <t>298 - 480</t>
-  </si>
-  <si>
-    <t>VSS</t>
-  </si>
-  <si>
-    <t>369 - 409</t>
+    <t>343 - 548</t>
   </si>
   <si>
     <t>Eagles</t>
   </si>
   <si>
-    <t>332 - 359</t>
+    <t>391 - 410</t>
   </si>
   <si>
     <t>ЛФК</t>
   </si>
   <si>
-    <t>343 - 433</t>
+    <t>394 - 492</t>
   </si>
   <si>
     <t>Минск 7х</t>
   </si>
   <si>
-    <t>300 - 401</t>
+    <t>329 - 469</t>
   </si>
   <si>
     <t>Стрела - Mapogo males 75:81 (16:30, БНТУ)</t>
@@ -259,6 +259,27 @@
   </si>
   <si>
     <t>NORD - SIRIUS 44:85 (15:30, БНТУ)</t>
+  </si>
+  <si>
+    <t>SIRIUS - ISsoft 67:53 (16:30, БНТУ)</t>
+  </si>
+  <si>
+    <t>Стрела - Грушвиль 59:76 (18:00, БНТУ)</t>
+  </si>
+  <si>
+    <t>Eagles - ЛФК 59:51 (19:30, БНТУ)</t>
+  </si>
+  <si>
+    <t>Минск 7х - VSS 29:68 (11:00, БНТУ)</t>
+  </si>
+  <si>
+    <t>GOLDEN HILL - NORD 68:45 (12:30, БНТУ)</t>
+  </si>
+  <si>
+    <t>Эра-Недвижимости плюс - БГУФК 89:92 (14:00, БНТУ)</t>
+  </si>
+  <si>
+    <t>Mapogo males - ОПЛАТИ 76:89 (15:30, БНТУ)</t>
   </si>
 </sst>
 </file>
@@ -714,8 +735,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D47066C-A84D-4953-AA40-17CF2279011C}">
-  <dimension ref="B2:H74"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C46A1EE0-58DA-414B-B37B-83274BF4E71B}">
+  <dimension ref="B2:H83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -770,10 +791,10 @@
         <v>8</v>
       </c>
       <c r="D5" s="3">
+        <v>7</v>
+      </c>
+      <c r="E5" s="3">
         <v>6</v>
-      </c>
-      <c r="E5" s="3">
-        <v>5</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -782,7 +803,7 @@
         <v>9</v>
       </c>
       <c r="H5" s="3">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -793,19 +814,19 @@
         <v>10</v>
       </c>
       <c r="D6" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E6" s="5">
         <v>5</v>
       </c>
       <c r="F6" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>11</v>
       </c>
       <c r="H6" s="5">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -816,19 +837,19 @@
         <v>12</v>
       </c>
       <c r="D7" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E7" s="5">
         <v>5</v>
       </c>
       <c r="F7" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H7" s="5">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -839,19 +860,19 @@
         <v>14</v>
       </c>
       <c r="D8" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E8" s="5">
         <v>5</v>
       </c>
       <c r="F8" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>15</v>
       </c>
       <c r="H8" s="5">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -862,10 +883,10 @@
         <v>16</v>
       </c>
       <c r="D9" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E9" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F9" s="5">
         <v>2</v>
@@ -874,7 +895,7 @@
         <v>17</v>
       </c>
       <c r="H9" s="5">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -885,10 +906,10 @@
         <v>18</v>
       </c>
       <c r="D10" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E10" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F10" s="5">
         <v>2</v>
@@ -897,7 +918,7 @@
         <v>19</v>
       </c>
       <c r="H10" s="5">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -908,10 +929,10 @@
         <v>20</v>
       </c>
       <c r="D11" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E11" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F11" s="5">
         <v>3</v>
@@ -920,7 +941,7 @@
         <v>21</v>
       </c>
       <c r="H11" s="5">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -931,10 +952,10 @@
         <v>22</v>
       </c>
       <c r="D12" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E12" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F12" s="5">
         <v>3</v>
@@ -943,7 +964,7 @@
         <v>23</v>
       </c>
       <c r="H12" s="5">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -954,10 +975,10 @@
         <v>24</v>
       </c>
       <c r="D13" s="7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E13" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F13" s="7">
         <v>4</v>
@@ -966,7 +987,7 @@
         <v>25</v>
       </c>
       <c r="H13" s="7">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -977,19 +998,19 @@
         <v>26</v>
       </c>
       <c r="D14" s="7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E14" s="7">
         <v>2</v>
       </c>
       <c r="F14" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G14" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H14" s="7">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1000,19 +1021,19 @@
         <v>28</v>
       </c>
       <c r="D15" s="7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E15" s="7">
         <v>2</v>
       </c>
       <c r="F15" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>29</v>
       </c>
       <c r="H15" s="7">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1023,10 +1044,10 @@
         <v>30</v>
       </c>
       <c r="D16" s="7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E16" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F16" s="7">
         <v>5</v>
@@ -1035,7 +1056,7 @@
         <v>31</v>
       </c>
       <c r="H16" s="7">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1046,19 +1067,19 @@
         <v>32</v>
       </c>
       <c r="D17" s="7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E17" s="7">
         <v>1</v>
       </c>
       <c r="F17" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>33</v>
       </c>
       <c r="H17" s="7">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1069,19 +1090,19 @@
         <v>34</v>
       </c>
       <c r="D18" s="7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E18" s="7">
         <v>0</v>
       </c>
       <c r="F18" s="7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H18" s="7">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
@@ -1689,10 +1710,118 @@
       <c r="G74" s="11"/>
       <c r="H74" s="11"/>
     </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B75" s="10">
+        <v>45654</v>
+      </c>
+      <c r="C75" s="9"/>
+      <c r="D75" s="9"/>
+      <c r="E75" s="9"/>
+      <c r="F75" s="9"/>
+      <c r="G75" s="9"/>
+      <c r="H75" s="9"/>
+    </row>
+    <row r="76" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B76" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C76" s="11"/>
+      <c r="D76" s="11"/>
+      <c r="E76" s="11"/>
+      <c r="F76" s="11"/>
+      <c r="G76" s="11"/>
+      <c r="H76" s="11"/>
+    </row>
+    <row r="77" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B77" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C77" s="11"/>
+      <c r="D77" s="11"/>
+      <c r="E77" s="11"/>
+      <c r="F77" s="11"/>
+      <c r="G77" s="11"/>
+      <c r="H77" s="11"/>
+    </row>
+    <row r="78" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B78" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C78" s="11"/>
+      <c r="D78" s="11"/>
+      <c r="E78" s="11"/>
+      <c r="F78" s="11"/>
+      <c r="G78" s="11"/>
+      <c r="H78" s="11"/>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B79" s="10">
+        <v>45655</v>
+      </c>
+      <c r="C79" s="9"/>
+      <c r="D79" s="9"/>
+      <c r="E79" s="9"/>
+      <c r="F79" s="9"/>
+      <c r="G79" s="9"/>
+      <c r="H79" s="9"/>
+    </row>
+    <row r="80" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B80" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C80" s="11"/>
+      <c r="D80" s="11"/>
+      <c r="E80" s="11"/>
+      <c r="F80" s="11"/>
+      <c r="G80" s="11"/>
+      <c r="H80" s="11"/>
+    </row>
+    <row r="81" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B81" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C81" s="11"/>
+      <c r="D81" s="11"/>
+      <c r="E81" s="11"/>
+      <c r="F81" s="11"/>
+      <c r="G81" s="11"/>
+      <c r="H81" s="11"/>
+    </row>
+    <row r="82" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B82" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C82" s="11"/>
+      <c r="D82" s="11"/>
+      <c r="E82" s="11"/>
+      <c r="F82" s="11"/>
+      <c r="G82" s="11"/>
+      <c r="H82" s="11"/>
+    </row>
+    <row r="83" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B83" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C83" s="11"/>
+      <c r="D83" s="11"/>
+      <c r="E83" s="11"/>
+      <c r="F83" s="11"/>
+      <c r="G83" s="11"/>
+      <c r="H83" s="11"/>
+    </row>
   </sheetData>
-  <mergeCells count="56">
+  <mergeCells count="65">
+    <mergeCell ref="B79:H79"/>
+    <mergeCell ref="B80:H80"/>
+    <mergeCell ref="B81:H81"/>
+    <mergeCell ref="B82:H82"/>
+    <mergeCell ref="B83:H83"/>
     <mergeCell ref="B73:H73"/>
     <mergeCell ref="B74:H74"/>
+    <mergeCell ref="B75:H75"/>
+    <mergeCell ref="B76:H76"/>
+    <mergeCell ref="B77:H77"/>
+    <mergeCell ref="B78:H78"/>
     <mergeCell ref="B67:H67"/>
     <mergeCell ref="B68:H68"/>
     <mergeCell ref="B69:H69"/>

</xml_diff>

<commit_message>
add stats vs VSS
</commit_message>
<xml_diff>
--- a/public/statistic/teams-position.xlsx
+++ b/public/statistic/teams-position.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Баскетбол\Отчёты\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{04DAFCBA-60C5-45F8-8143-6A53D88BE39D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{58AFBC64-890A-4FA3-8F2B-C9C4F086FA14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CE9FB605-9350-4803-900F-F452311DAEA1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E4FCB108-B8E9-45FA-80E2-722937BF3617}"/>
   </bookViews>
   <sheets>
     <sheet name="Д3" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <si>
     <t>Д3</t>
   </si>
@@ -51,88 +51,88 @@
     <t>Очки</t>
   </si>
   <si>
+    <t>ISsoft</t>
+  </si>
+  <si>
+    <t>515 - 438</t>
+  </si>
+  <si>
+    <t>Эра-Недвижимости плюс</t>
+  </si>
+  <si>
+    <t>604 - 497</t>
+  </si>
+  <si>
+    <t>ОПЛАТИ</t>
+  </si>
+  <si>
+    <t>573 - 514</t>
+  </si>
+  <si>
     <t>GOLDEN HILL</t>
   </si>
   <si>
-    <t>498 - 433</t>
-  </si>
-  <si>
-    <t>Эра-Недвижимости плюс</t>
-  </si>
-  <si>
-    <t>532 - 455</t>
-  </si>
-  <si>
-    <t>ISsoft</t>
-  </si>
-  <si>
-    <t>426 - 372</t>
-  </si>
-  <si>
-    <t>ОПЛАТИ</t>
-  </si>
-  <si>
-    <t>489 - 437</t>
+    <t>564 - 522</t>
   </si>
   <si>
     <t>Грушвиль</t>
   </si>
   <si>
-    <t>520 - 461</t>
+    <t>630 - 493</t>
   </si>
   <si>
     <t>Mapogo males</t>
   </si>
   <si>
-    <t>521 - 486</t>
+    <t>611 - 550</t>
   </si>
   <si>
     <t>БГУФК</t>
   </si>
   <si>
-    <t>497 - 412</t>
+    <t>569 - 456</t>
   </si>
   <si>
     <t>SIRIUS</t>
   </si>
   <si>
-    <t>458 - 391</t>
+    <t>542 - 434</t>
   </si>
   <si>
     <t>VSS</t>
   </si>
   <si>
-    <t>437 - 438</t>
+    <t>480 - 522</t>
   </si>
   <si>
     <t>Стрела</t>
   </si>
   <si>
-    <t>427 - 458</t>
+    <t>471 - 530</t>
   </si>
   <si>
     <t>NORD</t>
   </si>
   <si>
-    <t>343 - 548</t>
+    <t>407 - 638</t>
   </si>
   <si>
     <t>Eagles</t>
   </si>
   <si>
-    <t>391 - 410</t>
+    <t>468 - 494</t>
   </si>
   <si>
     <t>ЛФК</t>
   </si>
   <si>
-    <t>394 - 492</t>
+    <t>436 - 564</t>
   </si>
   <si>
     <t>Минск 7х</t>
   </si>
   <si>
-    <t>329 - 469</t>
+    <t>361 - 579</t>
   </si>
   <si>
     <t>Стрела - Mapogo males 75:81 (16:30, БНТУ)</t>
@@ -280,6 +280,27 @@
   </si>
   <si>
     <t>Mapogo males - ОПЛАТИ 76:89 (15:30, БНТУ)</t>
+  </si>
+  <si>
+    <t>Грушвиль - Минск 7х 110:32 (16:30, БНТУ)</t>
+  </si>
+  <si>
+    <t>БГУФК - Стрела 72:44 (18:00, БНТУ)</t>
+  </si>
+  <si>
+    <t>ОПЛАТИ - Eagles 84:77 (19:30, БНТУ)</t>
+  </si>
+  <si>
+    <t>VSS - SIRIUS 43:84 (11:00, БНТУ)</t>
+  </si>
+  <si>
+    <t>ISsoft - GOLDEN HILL 89:66 (12:30, БНТУ)</t>
+  </si>
+  <si>
+    <t>Эра-Недвижимости плюс - ЛФК 72:42 (14:00, БНТУ)</t>
+  </si>
+  <si>
+    <t>NORD - Mapogo males 64:90 (15:30, БНТУ)</t>
   </si>
 </sst>
 </file>
@@ -735,8 +756,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C46A1EE0-58DA-414B-B37B-83274BF4E71B}">
-  <dimension ref="B2:H83"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBC99850-61C8-4955-AEE6-57F3F741CDC9}">
+  <dimension ref="B2:H92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -791,19 +812,19 @@
         <v>8</v>
       </c>
       <c r="D5" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E5" s="3">
         <v>6</v>
       </c>
       <c r="F5" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="3">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -814,10 +835,10 @@
         <v>10</v>
       </c>
       <c r="D6" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E6" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F6" s="5">
         <v>2</v>
@@ -826,7 +847,7 @@
         <v>11</v>
       </c>
       <c r="H6" s="5">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -837,10 +858,10 @@
         <v>12</v>
       </c>
       <c r="D7" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E7" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F7" s="5">
         <v>2</v>
@@ -849,7 +870,7 @@
         <v>13</v>
       </c>
       <c r="H7" s="5">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -860,10 +881,10 @@
         <v>14</v>
       </c>
       <c r="D8" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E8" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F8" s="5">
         <v>2</v>
@@ -872,7 +893,7 @@
         <v>15</v>
       </c>
       <c r="H8" s="5">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -883,10 +904,10 @@
         <v>16</v>
       </c>
       <c r="D9" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E9" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F9" s="5">
         <v>2</v>
@@ -895,7 +916,7 @@
         <v>17</v>
       </c>
       <c r="H9" s="5">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -906,10 +927,10 @@
         <v>18</v>
       </c>
       <c r="D10" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E10" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F10" s="5">
         <v>2</v>
@@ -918,7 +939,7 @@
         <v>19</v>
       </c>
       <c r="H10" s="5">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -929,10 +950,10 @@
         <v>20</v>
       </c>
       <c r="D11" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E11" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F11" s="5">
         <v>3</v>
@@ -941,7 +962,7 @@
         <v>21</v>
       </c>
       <c r="H11" s="5">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -952,10 +973,10 @@
         <v>22</v>
       </c>
       <c r="D12" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E12" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F12" s="5">
         <v>3</v>
@@ -964,7 +985,7 @@
         <v>23</v>
       </c>
       <c r="H12" s="5">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -975,19 +996,19 @@
         <v>24</v>
       </c>
       <c r="D13" s="7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E13" s="7">
         <v>3</v>
       </c>
       <c r="F13" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>25</v>
       </c>
       <c r="H13" s="7">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -998,19 +1019,19 @@
         <v>26</v>
       </c>
       <c r="D14" s="7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E14" s="7">
         <v>2</v>
       </c>
       <c r="F14" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G14" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H14" s="7">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1021,19 +1042,19 @@
         <v>28</v>
       </c>
       <c r="D15" s="7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E15" s="7">
         <v>2</v>
       </c>
       <c r="F15" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>29</v>
       </c>
       <c r="H15" s="7">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1044,19 +1065,19 @@
         <v>30</v>
       </c>
       <c r="D16" s="7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E16" s="7">
         <v>2</v>
       </c>
       <c r="F16" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G16" s="7" t="s">
         <v>31</v>
       </c>
       <c r="H16" s="7">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1067,19 +1088,19 @@
         <v>32</v>
       </c>
       <c r="D17" s="7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E17" s="7">
         <v>1</v>
       </c>
       <c r="F17" s="7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>33</v>
       </c>
       <c r="H17" s="7">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1090,19 +1111,19 @@
         <v>34</v>
       </c>
       <c r="D18" s="7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E18" s="7">
         <v>0</v>
       </c>
       <c r="F18" s="7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H18" s="7">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
@@ -1809,13 +1830,121 @@
       <c r="G83" s="11"/>
       <c r="H83" s="11"/>
     </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B84" s="10">
+        <v>45675</v>
+      </c>
+      <c r="C84" s="9"/>
+      <c r="D84" s="9"/>
+      <c r="E84" s="9"/>
+      <c r="F84" s="9"/>
+      <c r="G84" s="9"/>
+      <c r="H84" s="9"/>
+    </row>
+    <row r="85" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B85" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C85" s="11"/>
+      <c r="D85" s="11"/>
+      <c r="E85" s="11"/>
+      <c r="F85" s="11"/>
+      <c r="G85" s="11"/>
+      <c r="H85" s="11"/>
+    </row>
+    <row r="86" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B86" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C86" s="11"/>
+      <c r="D86" s="11"/>
+      <c r="E86" s="11"/>
+      <c r="F86" s="11"/>
+      <c r="G86" s="11"/>
+      <c r="H86" s="11"/>
+    </row>
+    <row r="87" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B87" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C87" s="11"/>
+      <c r="D87" s="11"/>
+      <c r="E87" s="11"/>
+      <c r="F87" s="11"/>
+      <c r="G87" s="11"/>
+      <c r="H87" s="11"/>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B88" s="10">
+        <v>45676</v>
+      </c>
+      <c r="C88" s="9"/>
+      <c r="D88" s="9"/>
+      <c r="E88" s="9"/>
+      <c r="F88" s="9"/>
+      <c r="G88" s="9"/>
+      <c r="H88" s="9"/>
+    </row>
+    <row r="89" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B89" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C89" s="11"/>
+      <c r="D89" s="11"/>
+      <c r="E89" s="11"/>
+      <c r="F89" s="11"/>
+      <c r="G89" s="11"/>
+      <c r="H89" s="11"/>
+    </row>
+    <row r="90" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B90" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C90" s="11"/>
+      <c r="D90" s="11"/>
+      <c r="E90" s="11"/>
+      <c r="F90" s="11"/>
+      <c r="G90" s="11"/>
+      <c r="H90" s="11"/>
+    </row>
+    <row r="91" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B91" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C91" s="11"/>
+      <c r="D91" s="11"/>
+      <c r="E91" s="11"/>
+      <c r="F91" s="11"/>
+      <c r="G91" s="11"/>
+      <c r="H91" s="11"/>
+    </row>
+    <row r="92" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B92" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C92" s="11"/>
+      <c r="D92" s="11"/>
+      <c r="E92" s="11"/>
+      <c r="F92" s="11"/>
+      <c r="G92" s="11"/>
+      <c r="H92" s="11"/>
+    </row>
   </sheetData>
-  <mergeCells count="65">
+  <mergeCells count="74">
+    <mergeCell ref="B91:H91"/>
+    <mergeCell ref="B92:H92"/>
+    <mergeCell ref="B85:H85"/>
+    <mergeCell ref="B86:H86"/>
+    <mergeCell ref="B87:H87"/>
+    <mergeCell ref="B88:H88"/>
+    <mergeCell ref="B89:H89"/>
+    <mergeCell ref="B90:H90"/>
     <mergeCell ref="B79:H79"/>
     <mergeCell ref="B80:H80"/>
     <mergeCell ref="B81:H81"/>
     <mergeCell ref="B82:H82"/>
     <mergeCell ref="B83:H83"/>
+    <mergeCell ref="B84:H84"/>
     <mergeCell ref="B73:H73"/>
     <mergeCell ref="B74:H74"/>
     <mergeCell ref="B75:H75"/>

</xml_diff>

<commit_message>
add stats vs BGYfk
</commit_message>
<xml_diff>
--- a/public/statistic/teams-position.xlsx
+++ b/public/statistic/teams-position.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Баскетбол\Отчёты\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9674F1F6-FB02-4DE2-97BA-8E903FD680D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{286F14FD-CA22-40EF-B6E9-634E0A195E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6E419C2F-BA39-46F6-BA37-C1B29DCE64B3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8AFD9587-2588-479F-B0F8-426DF84F17E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Д3" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
     <t>Д3</t>
   </si>
@@ -54,85 +54,85 @@
     <t>ISsoft</t>
   </si>
   <si>
-    <t>584 - 490</t>
+    <t>653 - 532</t>
   </si>
   <si>
     <t>Эра-Недвижимости плюс</t>
   </si>
   <si>
-    <t>671 - 558</t>
+    <t>763 - 601</t>
   </si>
   <si>
     <t>ОПЛАТИ</t>
   </si>
   <si>
-    <t>671 - 571</t>
+    <t>756 - 616</t>
+  </si>
+  <si>
+    <t>GOLDEN HILL</t>
+  </si>
+  <si>
+    <t>728 - 668</t>
   </si>
   <si>
     <t>Грушвиль</t>
   </si>
   <si>
-    <t>725 - 572</t>
-  </si>
-  <si>
-    <t>GOLDEN HILL</t>
-  </si>
-  <si>
-    <t>643 - 588</t>
+    <t>805 - 657</t>
   </si>
   <si>
     <t>БГУФК</t>
   </si>
   <si>
-    <t>635 - 489</t>
+    <t>694 - 545</t>
   </si>
   <si>
     <t>Mapogo males</t>
   </si>
   <si>
-    <t>663 - 619</t>
+    <t>750 - 694</t>
   </si>
   <si>
     <t>SIRIUS</t>
   </si>
   <si>
-    <t>621 - 529</t>
+    <t>677 - 588</t>
+  </si>
+  <si>
+    <t>Стрела</t>
+  </si>
+  <si>
+    <t>600 - 655</t>
   </si>
   <si>
     <t>Eagles</t>
   </si>
   <si>
-    <t>536 - 550</t>
+    <t>578 - 619</t>
   </si>
   <si>
     <t>VSS</t>
   </si>
   <si>
-    <t>546 - 601</t>
+    <t>621 - 688</t>
   </si>
   <si>
     <t>NORD</t>
   </si>
   <si>
-    <t>463 - 706</t>
-  </si>
-  <si>
-    <t>Стрела</t>
-  </si>
-  <si>
-    <t>532 - 597</t>
+    <t>508 - 791</t>
   </si>
   <si>
     <t>ЛФК</t>
   </si>
   <si>
-    <t>493 - 662</t>
+    <t>551 - 730</t>
   </si>
   <si>
     <t>Минск 7х</t>
   </si>
   <si>
-    <t>394 - 645</t>
+    <t>437 - 737</t>
   </si>
   <si>
     <t>Стрела - Mapogo males 75:81 (16:30, БНТУ)</t>
@@ -322,6 +322,27 @@
   </si>
   <si>
     <t>ЛФК - ОПЛАТИ 57:98 (15:30, БНТУ)</t>
+  </si>
+  <si>
+    <t>ISsoft - Eagles 69:42 (16:30, БНТУ)</t>
+  </si>
+  <si>
+    <t>ЛФК - Стрела 58:68 (18:00, БНТУ)</t>
+  </si>
+  <si>
+    <t>VSS - Mapogo males 75:87 (19:30, БНТУ)</t>
+  </si>
+  <si>
+    <t>БГУФК - SIRIUS 59:56 (11:00, БНТУ)</t>
+  </si>
+  <si>
+    <t>Грушвиль - GOLDEN HILL 80:85 (12:30, БНТУ)</t>
+  </si>
+  <si>
+    <t>Эра-Недвижимости плюс - Минск 7х 92:43 (14:00, БНТУ)</t>
+  </si>
+  <si>
+    <t>NORD - ОПЛАТИ 45:85 (15:30, БНТУ)</t>
   </si>
 </sst>
 </file>
@@ -777,8 +798,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92B5F516-5F56-4195-A698-D7983AF302E6}">
-  <dimension ref="B2:H101"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF6E4830-8280-4C85-9C45-CBB844C1F5B7}">
+  <dimension ref="B2:H110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -833,10 +854,10 @@
         <v>8</v>
       </c>
       <c r="D5" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E5" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F5" s="3">
         <v>2</v>
@@ -845,7 +866,7 @@
         <v>9</v>
       </c>
       <c r="H5" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -856,10 +877,10 @@
         <v>10</v>
       </c>
       <c r="D6" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E6" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F6" s="5">
         <v>2</v>
@@ -868,7 +889,7 @@
         <v>11</v>
       </c>
       <c r="H6" s="5">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -879,10 +900,10 @@
         <v>12</v>
       </c>
       <c r="D7" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E7" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F7" s="5">
         <v>2</v>
@@ -891,7 +912,7 @@
         <v>13</v>
       </c>
       <c r="H7" s="5">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -902,10 +923,10 @@
         <v>14</v>
       </c>
       <c r="D8" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E8" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F8" s="5">
         <v>2</v>
@@ -914,7 +935,7 @@
         <v>15</v>
       </c>
       <c r="H8" s="5">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -925,19 +946,19 @@
         <v>16</v>
       </c>
       <c r="D9" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E9" s="5">
         <v>7</v>
       </c>
       <c r="F9" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>17</v>
       </c>
       <c r="H9" s="5">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -948,10 +969,10 @@
         <v>18</v>
       </c>
       <c r="D10" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E10" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F10" s="5">
         <v>3</v>
@@ -960,7 +981,7 @@
         <v>19</v>
       </c>
       <c r="H10" s="5">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -971,10 +992,10 @@
         <v>20</v>
       </c>
       <c r="D11" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E11" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F11" s="5">
         <v>3</v>
@@ -983,7 +1004,7 @@
         <v>21</v>
       </c>
       <c r="H11" s="5">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -994,19 +1015,19 @@
         <v>22</v>
       </c>
       <c r="D12" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E12" s="5">
         <v>5</v>
       </c>
       <c r="F12" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H12" s="5">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1017,19 +1038,19 @@
         <v>24</v>
       </c>
       <c r="D13" s="7">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E13" s="7">
         <v>3</v>
       </c>
       <c r="F13" s="7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>25</v>
       </c>
       <c r="H13" s="7">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1040,19 +1061,19 @@
         <v>26</v>
       </c>
       <c r="D14" s="7">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E14" s="7">
         <v>3</v>
       </c>
       <c r="F14" s="7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G14" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H14" s="7">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1063,10 +1084,10 @@
         <v>28</v>
       </c>
       <c r="D15" s="7">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E15" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F15" s="7">
         <v>7</v>
@@ -1075,7 +1096,7 @@
         <v>29</v>
       </c>
       <c r="H15" s="7">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1086,19 +1107,19 @@
         <v>30</v>
       </c>
       <c r="D16" s="7">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E16" s="7">
         <v>2</v>
       </c>
       <c r="F16" s="7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G16" s="7" t="s">
         <v>31</v>
       </c>
       <c r="H16" s="7">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1109,19 +1130,19 @@
         <v>32</v>
       </c>
       <c r="D17" s="7">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E17" s="7">
         <v>1</v>
       </c>
       <c r="F17" s="7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>33</v>
       </c>
       <c r="H17" s="7">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1132,19 +1153,19 @@
         <v>34</v>
       </c>
       <c r="D18" s="7">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E18" s="7">
         <v>0</v>
       </c>
       <c r="F18" s="7">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H18" s="7">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
@@ -2049,13 +2070,121 @@
       <c r="G101" s="11"/>
       <c r="H101" s="11"/>
     </row>
+    <row r="102" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B102" s="10">
+        <v>45703</v>
+      </c>
+      <c r="C102" s="9"/>
+      <c r="D102" s="9"/>
+      <c r="E102" s="9"/>
+      <c r="F102" s="9"/>
+      <c r="G102" s="9"/>
+      <c r="H102" s="9"/>
+    </row>
+    <row r="103" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B103" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C103" s="11"/>
+      <c r="D103" s="11"/>
+      <c r="E103" s="11"/>
+      <c r="F103" s="11"/>
+      <c r="G103" s="11"/>
+      <c r="H103" s="11"/>
+    </row>
+    <row r="104" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B104" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C104" s="11"/>
+      <c r="D104" s="11"/>
+      <c r="E104" s="11"/>
+      <c r="F104" s="11"/>
+      <c r="G104" s="11"/>
+      <c r="H104" s="11"/>
+    </row>
+    <row r="105" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B105" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C105" s="11"/>
+      <c r="D105" s="11"/>
+      <c r="E105" s="11"/>
+      <c r="F105" s="11"/>
+      <c r="G105" s="11"/>
+      <c r="H105" s="11"/>
+    </row>
+    <row r="106" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B106" s="10">
+        <v>45704</v>
+      </c>
+      <c r="C106" s="9"/>
+      <c r="D106" s="9"/>
+      <c r="E106" s="9"/>
+      <c r="F106" s="9"/>
+      <c r="G106" s="9"/>
+      <c r="H106" s="9"/>
+    </row>
+    <row r="107" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B107" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C107" s="11"/>
+      <c r="D107" s="11"/>
+      <c r="E107" s="11"/>
+      <c r="F107" s="11"/>
+      <c r="G107" s="11"/>
+      <c r="H107" s="11"/>
+    </row>
+    <row r="108" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B108" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C108" s="11"/>
+      <c r="D108" s="11"/>
+      <c r="E108" s="11"/>
+      <c r="F108" s="11"/>
+      <c r="G108" s="11"/>
+      <c r="H108" s="11"/>
+    </row>
+    <row r="109" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B109" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C109" s="11"/>
+      <c r="D109" s="11"/>
+      <c r="E109" s="11"/>
+      <c r="F109" s="11"/>
+      <c r="G109" s="11"/>
+      <c r="H109" s="11"/>
+    </row>
+    <row r="110" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B110" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C110" s="11"/>
+      <c r="D110" s="11"/>
+      <c r="E110" s="11"/>
+      <c r="F110" s="11"/>
+      <c r="G110" s="11"/>
+      <c r="H110" s="11"/>
+    </row>
   </sheetData>
-  <mergeCells count="83">
+  <mergeCells count="92">
+    <mergeCell ref="B109:H109"/>
+    <mergeCell ref="B110:H110"/>
+    <mergeCell ref="B103:H103"/>
+    <mergeCell ref="B104:H104"/>
+    <mergeCell ref="B105:H105"/>
+    <mergeCell ref="B106:H106"/>
+    <mergeCell ref="B107:H107"/>
+    <mergeCell ref="B108:H108"/>
     <mergeCell ref="B97:H97"/>
     <mergeCell ref="B98:H98"/>
     <mergeCell ref="B99:H99"/>
     <mergeCell ref="B100:H100"/>
     <mergeCell ref="B101:H101"/>
+    <mergeCell ref="B102:H102"/>
     <mergeCell ref="B91:H91"/>
     <mergeCell ref="B92:H92"/>
     <mergeCell ref="B93:H93"/>

</xml_diff>

<commit_message>
add stats vs Era Nedvizh
</commit_message>
<xml_diff>
--- a/public/statistic/teams-position.xlsx
+++ b/public/statistic/teams-position.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Баскетбол\Отчёты\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{286F14FD-CA22-40EF-B6E9-634E0A195E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E188A113-0AA1-4E22-9865-295BC4D0E391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8AFD9587-2588-479F-B0F8-426DF84F17E0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F9FF955C-21B0-43C0-AB24-A3F8E233D595}"/>
   </bookViews>
   <sheets>
     <sheet name="Д3" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
   <si>
     <t>Д3</t>
   </si>
@@ -54,85 +54,85 @@
     <t>ISsoft</t>
   </si>
   <si>
-    <t>653 - 532</t>
+    <t>725 - 586</t>
   </si>
   <si>
     <t>Эра-Недвижимости плюс</t>
   </si>
   <si>
-    <t>763 - 601</t>
+    <t>818 - 655</t>
+  </si>
+  <si>
+    <t>БГУФК</t>
+  </si>
+  <si>
+    <t>756 - 603</t>
+  </si>
+  <si>
+    <t>GOLDEN HILL</t>
+  </si>
+  <si>
+    <t>786 - 730</t>
+  </si>
+  <si>
+    <t>Грушвиль</t>
+  </si>
+  <si>
+    <t>905 - 738</t>
   </si>
   <si>
     <t>ОПЛАТИ</t>
   </si>
   <si>
-    <t>756 - 616</t>
-  </si>
-  <si>
-    <t>GOLDEN HILL</t>
-  </si>
-  <si>
-    <t>728 - 668</t>
-  </si>
-  <si>
-    <t>Грушвиль</t>
-  </si>
-  <si>
-    <t>805 - 657</t>
-  </si>
-  <si>
-    <t>БГУФК</t>
-  </si>
-  <si>
-    <t>694 - 545</t>
+    <t>810 - 688</t>
   </si>
   <si>
     <t>Mapogo males</t>
   </si>
   <si>
-    <t>750 - 694</t>
+    <t>831 - 794</t>
   </si>
   <si>
     <t>SIRIUS</t>
   </si>
   <si>
-    <t>677 - 588</t>
+    <t>731 - 643</t>
   </si>
   <si>
     <t>Стрела</t>
   </si>
   <si>
-    <t>600 - 655</t>
+    <t>671 - 705</t>
+  </si>
+  <si>
+    <t>VSS</t>
+  </si>
+  <si>
+    <t>689 - 746</t>
   </si>
   <si>
     <t>Eagles</t>
   </si>
   <si>
-    <t>578 - 619</t>
-  </si>
-  <si>
-    <t>VSS</t>
-  </si>
-  <si>
-    <t>621 - 688</t>
+    <t>636 - 687</t>
   </si>
   <si>
     <t>NORD</t>
   </si>
   <si>
-    <t>508 - 791</t>
+    <t>572 - 853</t>
   </si>
   <si>
     <t>ЛФК</t>
   </si>
   <si>
-    <t>551 - 730</t>
+    <t>613 - 794</t>
   </si>
   <si>
     <t>Минск 7х</t>
   </si>
   <si>
-    <t>437 - 737</t>
+    <t>487 - 808</t>
   </si>
   <si>
     <t>Стрела - Mapogo males 75:81 (16:30, БНТУ)</t>
@@ -343,6 +343,27 @@
   </si>
   <si>
     <t>NORD - ОПЛАТИ 45:85 (15:30, БНТУ)</t>
+  </si>
+  <si>
+    <t>Mapogo males - Грушвиль 81:100 (16:30, БНТУ)</t>
+  </si>
+  <si>
+    <t>Минск 7х - Стрела 50:71 (18:00, БНТУ)</t>
+  </si>
+  <si>
+    <t>ОПЛАТИ - ISsoft 54:72 (19:30, БНТУ)</t>
+  </si>
+  <si>
+    <t>NORD - ЛФК 64:62 (11:00, БНТУ)</t>
+  </si>
+  <si>
+    <t>SIRIUS - Эра-Недвижимости плюс 54:55 (12:30, БНТУ)</t>
+  </si>
+  <si>
+    <t>GOLDEN HILL - БГУФК 58:62 (14:00, БНТУ)</t>
+  </si>
+  <si>
+    <t>Eagles - VSS 58:68 (15:30, БНТУ)</t>
   </si>
 </sst>
 </file>
@@ -798,8 +819,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF6E4830-8280-4C85-9C45-CBB844C1F5B7}">
-  <dimension ref="B2:H110"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B325A8A-0004-4EF5-9EF1-C4CBED4E781F}">
+  <dimension ref="B2:H119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -854,10 +875,10 @@
         <v>8</v>
       </c>
       <c r="D5" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E5" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F5" s="3">
         <v>2</v>
@@ -866,7 +887,7 @@
         <v>9</v>
       </c>
       <c r="H5" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -877,10 +898,10 @@
         <v>10</v>
       </c>
       <c r="D6" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E6" s="5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F6" s="5">
         <v>2</v>
@@ -889,7 +910,7 @@
         <v>11</v>
       </c>
       <c r="H6" s="5">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -900,19 +921,19 @@
         <v>12</v>
       </c>
       <c r="D7" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E7" s="5">
         <v>8</v>
       </c>
       <c r="F7" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H7" s="5">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -923,19 +944,19 @@
         <v>14</v>
       </c>
       <c r="D8" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E8" s="5">
         <v>8</v>
       </c>
       <c r="F8" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>15</v>
       </c>
       <c r="H8" s="5">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -946,10 +967,10 @@
         <v>16</v>
       </c>
       <c r="D9" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E9" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F9" s="5">
         <v>3</v>
@@ -958,7 +979,7 @@
         <v>17</v>
       </c>
       <c r="H9" s="5">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -969,10 +990,10 @@
         <v>18</v>
       </c>
       <c r="D10" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E10" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F10" s="5">
         <v>3</v>
@@ -981,7 +1002,7 @@
         <v>19</v>
       </c>
       <c r="H10" s="5">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -992,19 +1013,19 @@
         <v>20</v>
       </c>
       <c r="D11" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E11" s="5">
         <v>7</v>
       </c>
       <c r="F11" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>21</v>
       </c>
       <c r="H11" s="5">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1015,19 +1036,19 @@
         <v>22</v>
       </c>
       <c r="D12" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E12" s="5">
         <v>5</v>
       </c>
       <c r="F12" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H12" s="5">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1038,10 +1059,10 @@
         <v>24</v>
       </c>
       <c r="D13" s="7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E13" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F13" s="7">
         <v>7</v>
@@ -1050,7 +1071,7 @@
         <v>25</v>
       </c>
       <c r="H13" s="7">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1061,10 +1082,10 @@
         <v>26</v>
       </c>
       <c r="D14" s="7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E14" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F14" s="7">
         <v>7</v>
@@ -1073,7 +1094,7 @@
         <v>27</v>
       </c>
       <c r="H14" s="7">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1084,19 +1105,19 @@
         <v>28</v>
       </c>
       <c r="D15" s="7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E15" s="7">
         <v>3</v>
       </c>
       <c r="F15" s="7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>29</v>
       </c>
       <c r="H15" s="7">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1107,10 +1128,10 @@
         <v>30</v>
       </c>
       <c r="D16" s="7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E16" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F16" s="7">
         <v>8</v>
@@ -1119,7 +1140,7 @@
         <v>31</v>
       </c>
       <c r="H16" s="7">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1130,19 +1151,19 @@
         <v>32</v>
       </c>
       <c r="D17" s="7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E17" s="7">
         <v>1</v>
       </c>
       <c r="F17" s="7">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>33</v>
       </c>
       <c r="H17" s="7">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1153,19 +1174,19 @@
         <v>34</v>
       </c>
       <c r="D18" s="7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E18" s="7">
         <v>0</v>
       </c>
       <c r="F18" s="7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H18" s="7">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
@@ -2169,10 +2190,118 @@
       <c r="G110" s="11"/>
       <c r="H110" s="11"/>
     </row>
+    <row r="111" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B111" s="10">
+        <v>45717</v>
+      </c>
+      <c r="C111" s="9"/>
+      <c r="D111" s="9"/>
+      <c r="E111" s="9"/>
+      <c r="F111" s="9"/>
+      <c r="G111" s="9"/>
+      <c r="H111" s="9"/>
+    </row>
+    <row r="112" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B112" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C112" s="11"/>
+      <c r="D112" s="11"/>
+      <c r="E112" s="11"/>
+      <c r="F112" s="11"/>
+      <c r="G112" s="11"/>
+      <c r="H112" s="11"/>
+    </row>
+    <row r="113" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B113" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C113" s="11"/>
+      <c r="D113" s="11"/>
+      <c r="E113" s="11"/>
+      <c r="F113" s="11"/>
+      <c r="G113" s="11"/>
+      <c r="H113" s="11"/>
+    </row>
+    <row r="114" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B114" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C114" s="11"/>
+      <c r="D114" s="11"/>
+      <c r="E114" s="11"/>
+      <c r="F114" s="11"/>
+      <c r="G114" s="11"/>
+      <c r="H114" s="11"/>
+    </row>
+    <row r="115" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B115" s="10">
+        <v>45718</v>
+      </c>
+      <c r="C115" s="9"/>
+      <c r="D115" s="9"/>
+      <c r="E115" s="9"/>
+      <c r="F115" s="9"/>
+      <c r="G115" s="9"/>
+      <c r="H115" s="9"/>
+    </row>
+    <row r="116" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B116" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C116" s="11"/>
+      <c r="D116" s="11"/>
+      <c r="E116" s="11"/>
+      <c r="F116" s="11"/>
+      <c r="G116" s="11"/>
+      <c r="H116" s="11"/>
+    </row>
+    <row r="117" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B117" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C117" s="11"/>
+      <c r="D117" s="11"/>
+      <c r="E117" s="11"/>
+      <c r="F117" s="11"/>
+      <c r="G117" s="11"/>
+      <c r="H117" s="11"/>
+    </row>
+    <row r="118" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B118" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C118" s="11"/>
+      <c r="D118" s="11"/>
+      <c r="E118" s="11"/>
+      <c r="F118" s="11"/>
+      <c r="G118" s="11"/>
+      <c r="H118" s="11"/>
+    </row>
+    <row r="119" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B119" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="C119" s="11"/>
+      <c r="D119" s="11"/>
+      <c r="E119" s="11"/>
+      <c r="F119" s="11"/>
+      <c r="G119" s="11"/>
+      <c r="H119" s="11"/>
+    </row>
   </sheetData>
-  <mergeCells count="92">
+  <mergeCells count="101">
+    <mergeCell ref="B115:H115"/>
+    <mergeCell ref="B116:H116"/>
+    <mergeCell ref="B117:H117"/>
+    <mergeCell ref="B118:H118"/>
+    <mergeCell ref="B119:H119"/>
     <mergeCell ref="B109:H109"/>
     <mergeCell ref="B110:H110"/>
+    <mergeCell ref="B111:H111"/>
+    <mergeCell ref="B112:H112"/>
+    <mergeCell ref="B113:H113"/>
+    <mergeCell ref="B114:H114"/>
     <mergeCell ref="B103:H103"/>
     <mergeCell ref="B104:H104"/>
     <mergeCell ref="B105:H105"/>

</xml_diff>

<commit_message>
add stats vs Strela
</commit_message>
<xml_diff>
--- a/public/statistic/teams-position.xlsx
+++ b/public/statistic/teams-position.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Баскетбол\Отчёты\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E188A113-0AA1-4E22-9865-295BC4D0E391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{67554D83-ABA5-4B08-8B5B-64E109F0E95F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F9FF955C-21B0-43C0-AB24-A3F8E233D595}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7FECC818-F17C-4789-897C-BF5B26E7CC77}"/>
   </bookViews>
   <sheets>
     <sheet name="Д3" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
   <si>
     <t>Д3</t>
   </si>
@@ -54,85 +54,85 @@
     <t>ISsoft</t>
   </si>
   <si>
-    <t>725 - 586</t>
+    <t>818 - 660</t>
   </si>
   <si>
     <t>Эра-Недвижимости плюс</t>
   </si>
   <si>
-    <t>818 - 655</t>
+    <t>892 - 720</t>
   </si>
   <si>
     <t>БГУФК</t>
   </si>
   <si>
-    <t>756 - 603</t>
+    <t>835 - 668</t>
+  </si>
+  <si>
+    <t>Грушвиль</t>
+  </si>
+  <si>
+    <t>973 - 788</t>
+  </si>
+  <si>
+    <t>ОПЛАТИ</t>
+  </si>
+  <si>
+    <t>901 - 726</t>
   </si>
   <si>
     <t>GOLDEN HILL</t>
   </si>
   <si>
-    <t>786 - 730</t>
-  </si>
-  <si>
-    <t>Грушвиль</t>
-  </si>
-  <si>
-    <t>905 - 738</t>
-  </si>
-  <si>
-    <t>ОПЛАТИ</t>
-  </si>
-  <si>
-    <t>810 - 688</t>
+    <t>851 - 804</t>
   </si>
   <si>
     <t>Mapogo males</t>
   </si>
   <si>
-    <t>831 - 794</t>
+    <t>896 - 873</t>
   </si>
   <si>
     <t>SIRIUS</t>
   </si>
   <si>
-    <t>731 - 643</t>
+    <t>798 - 695</t>
   </si>
   <si>
     <t>Стрела</t>
   </si>
   <si>
-    <t>671 - 705</t>
+    <t>723 - 772</t>
   </si>
   <si>
     <t>VSS</t>
   </si>
   <si>
-    <t>689 - 746</t>
+    <t>727 - 837</t>
   </si>
   <si>
     <t>Eagles</t>
   </si>
   <si>
-    <t>636 - 687</t>
+    <t>686 - 755</t>
   </si>
   <si>
     <t>NORD</t>
   </si>
   <si>
-    <t>572 - 853</t>
+    <t>646 - 946</t>
   </si>
   <si>
     <t>ЛФК</t>
   </si>
   <si>
-    <t>613 - 794</t>
+    <t>676 - 831</t>
   </si>
   <si>
     <t>Минск 7х</t>
   </si>
   <si>
-    <t>487 - 808</t>
+    <t>524 - 871</t>
   </si>
   <si>
     <t>Стрела - Mapogo males 75:81 (16:30, БНТУ)</t>
@@ -364,6 +364,27 @@
   </si>
   <si>
     <t>Eagles - VSS 58:68 (15:30, БНТУ)</t>
+  </si>
+  <si>
+    <t>БГУФК - Mapogo males 79:65 (16:30, БНТУ)</t>
+  </si>
+  <si>
+    <t>Минск 7х - ЛФК 37:63 (18:00, БНТУ)</t>
+  </si>
+  <si>
+    <t>Грушвиль - Eagles 68:50 (19:30, БНТУ)</t>
+  </si>
+  <si>
+    <t>ISsoft - NORD 93:74 (11:00, БНТУ)</t>
+  </si>
+  <si>
+    <t>Стрела - SIRIUS 52:67 (12:30, БНТУ)</t>
+  </si>
+  <si>
+    <t>Эра-Недвижимости плюс - GOLDEN HILL 74:65 (14:00, БНТУ)</t>
+  </si>
+  <si>
+    <t>VSS - ОПЛАТИ 38:91 (15:30, БНТУ)</t>
   </si>
 </sst>
 </file>
@@ -819,8 +840,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B325A8A-0004-4EF5-9EF1-C4CBED4E781F}">
-  <dimension ref="B2:H119"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8638D96-D238-4FBF-9C27-D1A6C8F59957}">
+  <dimension ref="B2:H128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -875,10 +896,10 @@
         <v>8</v>
       </c>
       <c r="D5" s="3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E5" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F5" s="3">
         <v>2</v>
@@ -887,7 +908,7 @@
         <v>9</v>
       </c>
       <c r="H5" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -898,10 +919,10 @@
         <v>10</v>
       </c>
       <c r="D6" s="5">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E6" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F6" s="5">
         <v>2</v>
@@ -910,7 +931,7 @@
         <v>11</v>
       </c>
       <c r="H6" s="5">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -921,10 +942,10 @@
         <v>12</v>
       </c>
       <c r="D7" s="5">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E7" s="5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F7" s="5">
         <v>3</v>
@@ -933,7 +954,7 @@
         <v>13</v>
       </c>
       <c r="H7" s="5">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -944,10 +965,10 @@
         <v>14</v>
       </c>
       <c r="D8" s="5">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E8" s="5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F8" s="5">
         <v>3</v>
@@ -956,7 +977,7 @@
         <v>15</v>
       </c>
       <c r="H8" s="5">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -967,10 +988,10 @@
         <v>16</v>
       </c>
       <c r="D9" s="5">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E9" s="5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F9" s="5">
         <v>3</v>
@@ -979,7 +1000,7 @@
         <v>17</v>
       </c>
       <c r="H9" s="5">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -990,19 +1011,19 @@
         <v>18</v>
       </c>
       <c r="D10" s="5">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E10" s="5">
         <v>8</v>
       </c>
       <c r="F10" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H10" s="5">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1013,19 +1034,19 @@
         <v>20</v>
       </c>
       <c r="D11" s="5">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E11" s="5">
         <v>7</v>
       </c>
       <c r="F11" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>21</v>
       </c>
       <c r="H11" s="5">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1036,10 +1057,10 @@
         <v>22</v>
       </c>
       <c r="D12" s="5">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E12" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F12" s="5">
         <v>6</v>
@@ -1048,7 +1069,7 @@
         <v>23</v>
       </c>
       <c r="H12" s="5">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1059,19 +1080,19 @@
         <v>24</v>
       </c>
       <c r="D13" s="7">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E13" s="7">
         <v>4</v>
       </c>
       <c r="F13" s="7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>25</v>
       </c>
       <c r="H13" s="7">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1082,19 +1103,19 @@
         <v>26</v>
       </c>
       <c r="D14" s="7">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E14" s="7">
         <v>4</v>
       </c>
       <c r="F14" s="7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G14" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H14" s="7">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1105,19 +1126,19 @@
         <v>28</v>
       </c>
       <c r="D15" s="7">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E15" s="7">
         <v>3</v>
       </c>
       <c r="F15" s="7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>29</v>
       </c>
       <c r="H15" s="7">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1128,19 +1149,19 @@
         <v>30</v>
       </c>
       <c r="D16" s="7">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E16" s="7">
         <v>3</v>
       </c>
       <c r="F16" s="7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G16" s="7" t="s">
         <v>31</v>
       </c>
       <c r="H16" s="7">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1151,10 +1172,10 @@
         <v>32</v>
       </c>
       <c r="D17" s="7">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E17" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F17" s="7">
         <v>10</v>
@@ -1163,7 +1184,7 @@
         <v>33</v>
       </c>
       <c r="H17" s="7">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1174,19 +1195,19 @@
         <v>34</v>
       </c>
       <c r="D18" s="7">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E18" s="7">
         <v>0</v>
       </c>
       <c r="F18" s="7">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H18" s="7">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
@@ -2289,13 +2310,121 @@
       <c r="G119" s="11"/>
       <c r="H119" s="11"/>
     </row>
+    <row r="120" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B120" s="10">
+        <v>45731</v>
+      </c>
+      <c r="C120" s="9"/>
+      <c r="D120" s="9"/>
+      <c r="E120" s="9"/>
+      <c r="F120" s="9"/>
+      <c r="G120" s="9"/>
+      <c r="H120" s="9"/>
+    </row>
+    <row r="121" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B121" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C121" s="11"/>
+      <c r="D121" s="11"/>
+      <c r="E121" s="11"/>
+      <c r="F121" s="11"/>
+      <c r="G121" s="11"/>
+      <c r="H121" s="11"/>
+    </row>
+    <row r="122" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B122" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C122" s="11"/>
+      <c r="D122" s="11"/>
+      <c r="E122" s="11"/>
+      <c r="F122" s="11"/>
+      <c r="G122" s="11"/>
+      <c r="H122" s="11"/>
+    </row>
+    <row r="123" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B123" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C123" s="11"/>
+      <c r="D123" s="11"/>
+      <c r="E123" s="11"/>
+      <c r="F123" s="11"/>
+      <c r="G123" s="11"/>
+      <c r="H123" s="11"/>
+    </row>
+    <row r="124" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B124" s="10">
+        <v>45732</v>
+      </c>
+      <c r="C124" s="9"/>
+      <c r="D124" s="9"/>
+      <c r="E124" s="9"/>
+      <c r="F124" s="9"/>
+      <c r="G124" s="9"/>
+      <c r="H124" s="9"/>
+    </row>
+    <row r="125" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B125" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C125" s="11"/>
+      <c r="D125" s="11"/>
+      <c r="E125" s="11"/>
+      <c r="F125" s="11"/>
+      <c r="G125" s="11"/>
+      <c r="H125" s="11"/>
+    </row>
+    <row r="126" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B126" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C126" s="11"/>
+      <c r="D126" s="11"/>
+      <c r="E126" s="11"/>
+      <c r="F126" s="11"/>
+      <c r="G126" s="11"/>
+      <c r="H126" s="11"/>
+    </row>
+    <row r="127" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B127" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C127" s="11"/>
+      <c r="D127" s="11"/>
+      <c r="E127" s="11"/>
+      <c r="F127" s="11"/>
+      <c r="G127" s="11"/>
+      <c r="H127" s="11"/>
+    </row>
+    <row r="128" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B128" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C128" s="11"/>
+      <c r="D128" s="11"/>
+      <c r="E128" s="11"/>
+      <c r="F128" s="11"/>
+      <c r="G128" s="11"/>
+      <c r="H128" s="11"/>
+    </row>
   </sheetData>
-  <mergeCells count="101">
+  <mergeCells count="110">
+    <mergeCell ref="B127:H127"/>
+    <mergeCell ref="B128:H128"/>
+    <mergeCell ref="B121:H121"/>
+    <mergeCell ref="B122:H122"/>
+    <mergeCell ref="B123:H123"/>
+    <mergeCell ref="B124:H124"/>
+    <mergeCell ref="B125:H125"/>
+    <mergeCell ref="B126:H126"/>
     <mergeCell ref="B115:H115"/>
     <mergeCell ref="B116:H116"/>
     <mergeCell ref="B117:H117"/>
     <mergeCell ref="B118:H118"/>
     <mergeCell ref="B119:H119"/>
+    <mergeCell ref="B120:H120"/>
     <mergeCell ref="B109:H109"/>
     <mergeCell ref="B110:H110"/>
     <mergeCell ref="B111:H111"/>

</xml_diff>

<commit_message>
add stats vs Minsk7x
</commit_message>
<xml_diff>
--- a/public/statistic/teams-position.xlsx
+++ b/public/statistic/teams-position.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Баскетбол\Отчёты\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67554D83-ABA5-4B08-8B5B-64E109F0E95F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4CED39D4-0FE6-4B94-BEB9-AC148E1B3BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7FECC818-F17C-4789-897C-BF5B26E7CC77}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{27E01D56-B4F6-4552-98CF-7634B539AC83}"/>
   </bookViews>
   <sheets>
     <sheet name="Д3" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="127">
   <si>
     <t>Д3</t>
   </si>
@@ -54,85 +54,85 @@
     <t>ISsoft</t>
   </si>
   <si>
-    <t>818 - 660</t>
+    <t>885 - 719</t>
+  </si>
+  <si>
+    <t>БГУФК</t>
+  </si>
+  <si>
+    <t>897 - 724</t>
   </si>
   <si>
     <t>Эра-Недвижимости плюс</t>
   </si>
   <si>
-    <t>892 - 720</t>
-  </si>
-  <si>
-    <t>БГУФК</t>
-  </si>
-  <si>
-    <t>835 - 668</t>
+    <t>956 - 801</t>
+  </si>
+  <si>
+    <t>ОПЛАТИ</t>
+  </si>
+  <si>
+    <t>985 - 806</t>
+  </si>
+  <si>
+    <t>GOLDEN HILL</t>
+  </si>
+  <si>
+    <t>930 - 865</t>
   </si>
   <si>
     <t>Грушвиль</t>
   </si>
   <si>
-    <t>973 - 788</t>
-  </si>
-  <si>
-    <t>ОПЛАТИ</t>
-  </si>
-  <si>
-    <t>901 - 726</t>
-  </si>
-  <si>
-    <t>GOLDEN HILL</t>
-  </si>
-  <si>
-    <t>851 - 804</t>
+    <t>1053 - 872</t>
   </si>
   <si>
     <t>Mapogo males</t>
   </si>
   <si>
-    <t>896 - 873</t>
+    <t>977 - 937</t>
   </si>
   <si>
     <t>SIRIUS</t>
   </si>
   <si>
-    <t>798 - 695</t>
+    <t>876 - 743</t>
+  </si>
+  <si>
+    <t>VSS</t>
+  </si>
+  <si>
+    <t>797 - 904</t>
   </si>
   <si>
     <t>Стрела</t>
   </si>
   <si>
-    <t>723 - 772</t>
-  </si>
-  <si>
-    <t>VSS</t>
-  </si>
-  <si>
-    <t>727 - 837</t>
+    <t>784 - 851</t>
   </si>
   <si>
     <t>Eagles</t>
   </si>
   <si>
-    <t>686 - 755</t>
+    <t>742 - 817</t>
   </si>
   <si>
     <t>NORD</t>
   </si>
   <si>
-    <t>646 - 946</t>
+    <t>713 - 1016</t>
   </si>
   <si>
     <t>ЛФК</t>
   </si>
   <si>
-    <t>676 - 831</t>
+    <t>735 - 898</t>
   </si>
   <si>
     <t>Минск 7х</t>
   </si>
   <si>
-    <t>524 - 871</t>
+    <t>572 - 949</t>
   </si>
   <si>
     <t>Стрела - Mapogo males 75:81 (16:30, БНТУ)</t>
@@ -385,6 +385,27 @@
   </si>
   <si>
     <t>VSS - ОПЛАТИ 38:91 (15:30, БНТУ)</t>
+  </si>
+  <si>
+    <t>ЛФК - ISsoft 59:67 (16:30, БНТУ)</t>
+  </si>
+  <si>
+    <t>ОПЛАТИ - Грушвиль 84:80 (18:00, БНТУ)</t>
+  </si>
+  <si>
+    <t>Eagles - БГУФК 56:62 (19:30, БНТУ)</t>
+  </si>
+  <si>
+    <t>NORD - VSS 67:70 (11:00, БНТУ)</t>
+  </si>
+  <si>
+    <t>SIRIUS - Минск 7х 78:48 (12:30, БНТУ)</t>
+  </si>
+  <si>
+    <t>Эра-Недвижимости плюс - Mapogo males 64:81 (14:00, БНТУ)</t>
+  </si>
+  <si>
+    <t>GOLDEN HILL - Стрела 79:61 (15:30, БНТУ)</t>
   </si>
 </sst>
 </file>
@@ -840,8 +861,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8638D96-D238-4FBF-9C27-D1A6C8F59957}">
-  <dimension ref="B2:H128"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED2A38AD-E23B-4D69-9515-7F293D47ACF9}">
+  <dimension ref="B2:H137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -896,10 +917,10 @@
         <v>8</v>
       </c>
       <c r="D5" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E5" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F5" s="3">
         <v>2</v>
@@ -908,7 +929,7 @@
         <v>9</v>
       </c>
       <c r="H5" s="3">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -919,19 +940,19 @@
         <v>10</v>
       </c>
       <c r="D6" s="5">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E6" s="5">
         <v>10</v>
       </c>
       <c r="F6" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>11</v>
       </c>
       <c r="H6" s="5">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -942,10 +963,10 @@
         <v>12</v>
       </c>
       <c r="D7" s="5">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E7" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F7" s="5">
         <v>3</v>
@@ -954,7 +975,7 @@
         <v>13</v>
       </c>
       <c r="H7" s="5">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -965,10 +986,10 @@
         <v>14</v>
       </c>
       <c r="D8" s="5">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E8" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F8" s="5">
         <v>3</v>
@@ -977,7 +998,7 @@
         <v>15</v>
       </c>
       <c r="H8" s="5">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -988,19 +1009,19 @@
         <v>16</v>
       </c>
       <c r="D9" s="5">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E9" s="5">
         <v>9</v>
       </c>
       <c r="F9" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>17</v>
       </c>
       <c r="H9" s="5">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1011,10 +1032,10 @@
         <v>18</v>
       </c>
       <c r="D10" s="5">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E10" s="5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F10" s="5">
         <v>4</v>
@@ -1023,7 +1044,7 @@
         <v>19</v>
       </c>
       <c r="H10" s="5">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1034,10 +1055,10 @@
         <v>20</v>
       </c>
       <c r="D11" s="5">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E11" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F11" s="5">
         <v>5</v>
@@ -1046,7 +1067,7 @@
         <v>21</v>
       </c>
       <c r="H11" s="5">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1057,10 +1078,10 @@
         <v>22</v>
       </c>
       <c r="D12" s="5">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E12" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F12" s="5">
         <v>6</v>
@@ -1069,7 +1090,7 @@
         <v>23</v>
       </c>
       <c r="H12" s="5">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1080,10 +1101,10 @@
         <v>24</v>
       </c>
       <c r="D13" s="7">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E13" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F13" s="7">
         <v>8</v>
@@ -1092,7 +1113,7 @@
         <v>25</v>
       </c>
       <c r="H13" s="7">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1103,19 +1124,19 @@
         <v>26</v>
       </c>
       <c r="D14" s="7">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E14" s="7">
         <v>4</v>
       </c>
       <c r="F14" s="7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G14" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H14" s="7">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1126,19 +1147,19 @@
         <v>28</v>
       </c>
       <c r="D15" s="7">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E15" s="7">
         <v>3</v>
       </c>
       <c r="F15" s="7">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>29</v>
       </c>
       <c r="H15" s="7">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1149,19 +1170,19 @@
         <v>30</v>
       </c>
       <c r="D16" s="7">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E16" s="7">
         <v>3</v>
       </c>
       <c r="F16" s="7">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G16" s="7" t="s">
         <v>31</v>
       </c>
       <c r="H16" s="7">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1172,19 +1193,19 @@
         <v>32</v>
       </c>
       <c r="D17" s="7">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E17" s="7">
         <v>2</v>
       </c>
       <c r="F17" s="7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>33</v>
       </c>
       <c r="H17" s="7">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1195,19 +1216,19 @@
         <v>34</v>
       </c>
       <c r="D18" s="7">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E18" s="7">
         <v>0</v>
       </c>
       <c r="F18" s="7">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H18" s="7">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
@@ -2409,10 +2430,118 @@
       <c r="G128" s="11"/>
       <c r="H128" s="11"/>
     </row>
+    <row r="129" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B129" s="10">
+        <v>45745</v>
+      </c>
+      <c r="C129" s="9"/>
+      <c r="D129" s="9"/>
+      <c r="E129" s="9"/>
+      <c r="F129" s="9"/>
+      <c r="G129" s="9"/>
+      <c r="H129" s="9"/>
+    </row>
+    <row r="130" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B130" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C130" s="11"/>
+      <c r="D130" s="11"/>
+      <c r="E130" s="11"/>
+      <c r="F130" s="11"/>
+      <c r="G130" s="11"/>
+      <c r="H130" s="11"/>
+    </row>
+    <row r="131" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B131" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C131" s="11"/>
+      <c r="D131" s="11"/>
+      <c r="E131" s="11"/>
+      <c r="F131" s="11"/>
+      <c r="G131" s="11"/>
+      <c r="H131" s="11"/>
+    </row>
+    <row r="132" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B132" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C132" s="11"/>
+      <c r="D132" s="11"/>
+      <c r="E132" s="11"/>
+      <c r="F132" s="11"/>
+      <c r="G132" s="11"/>
+      <c r="H132" s="11"/>
+    </row>
+    <row r="133" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B133" s="10">
+        <v>45746</v>
+      </c>
+      <c r="C133" s="9"/>
+      <c r="D133" s="9"/>
+      <c r="E133" s="9"/>
+      <c r="F133" s="9"/>
+      <c r="G133" s="9"/>
+      <c r="H133" s="9"/>
+    </row>
+    <row r="134" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B134" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C134" s="11"/>
+      <c r="D134" s="11"/>
+      <c r="E134" s="11"/>
+      <c r="F134" s="11"/>
+      <c r="G134" s="11"/>
+      <c r="H134" s="11"/>
+    </row>
+    <row r="135" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B135" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C135" s="11"/>
+      <c r="D135" s="11"/>
+      <c r="E135" s="11"/>
+      <c r="F135" s="11"/>
+      <c r="G135" s="11"/>
+      <c r="H135" s="11"/>
+    </row>
+    <row r="136" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B136" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C136" s="11"/>
+      <c r="D136" s="11"/>
+      <c r="E136" s="11"/>
+      <c r="F136" s="11"/>
+      <c r="G136" s="11"/>
+      <c r="H136" s="11"/>
+    </row>
+    <row r="137" spans="2:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B137" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C137" s="11"/>
+      <c r="D137" s="11"/>
+      <c r="E137" s="11"/>
+      <c r="F137" s="11"/>
+      <c r="G137" s="11"/>
+      <c r="H137" s="11"/>
+    </row>
   </sheetData>
-  <mergeCells count="110">
+  <mergeCells count="119">
+    <mergeCell ref="B133:H133"/>
+    <mergeCell ref="B134:H134"/>
+    <mergeCell ref="B135:H135"/>
+    <mergeCell ref="B136:H136"/>
+    <mergeCell ref="B137:H137"/>
     <mergeCell ref="B127:H127"/>
     <mergeCell ref="B128:H128"/>
+    <mergeCell ref="B129:H129"/>
+    <mergeCell ref="B130:H130"/>
+    <mergeCell ref="B131:H131"/>
+    <mergeCell ref="B132:H132"/>
     <mergeCell ref="B121:H121"/>
     <mergeCell ref="B122:H122"/>
     <mergeCell ref="B123:H123"/>

</xml_diff>